<commit_message>
Final xlsx additions and typo fix
</commit_message>
<xml_diff>
--- a/Project Files/Data Files/Amazon_DDT_Excel/Katlon_VIP_TC_Varshith.xlsx
+++ b/Project Files/Data Files/Amazon_DDT_Excel/Katlon_VIP_TC_Varshith.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\puliv\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B858560E-F0FC-4F4F-B12C-834F191A33AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B04023B3-7E5D-4059-A1A1-27F3A16F76DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="6" xr2:uid="{180CE421-F235-4C01-B743-0C744B666E43}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{180CE421-F235-4C01-B743-0C744B666E43}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="125">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -261,12 +261,6 @@
     <t>Proceed to check out</t>
   </si>
   <si>
-    <t>Validate the amazon application for the Sign In User Interface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validate the amazon application to Add an item to Cart </t>
-  </si>
-  <si>
     <t>Electronics, Smart Watches</t>
   </si>
   <si>
@@ -334,6 +328,84 @@
   </si>
   <si>
     <t>Lotions</t>
+  </si>
+  <si>
+    <t>TC_Amazon_Registration_001</t>
+  </si>
+  <si>
+    <t>TC_Amazon_Sign In_002</t>
+  </si>
+  <si>
+    <t>TC_Amazon_Search_003</t>
+  </si>
+  <si>
+    <t>TC_Amazon_Add to Cart_004</t>
+  </si>
+  <si>
+    <t>TC_Amazon_Orders_005</t>
+  </si>
+  <si>
+    <t>Validate the amazon application to Order an item</t>
+  </si>
+  <si>
+    <t>TC_Amzon_Change Language_006</t>
+  </si>
+  <si>
+    <t>Validate the amazon application to Change Langugae</t>
+  </si>
+  <si>
+    <t>TC_Amazon_Try Prime_007</t>
+  </si>
+  <si>
+    <t>Validate the amazon application to Try Prime Subscription</t>
+  </si>
+  <si>
+    <t>TC_Amzon_Browding History_008</t>
+  </si>
+  <si>
+    <t>Validate the amazon application for Browsing Histroy</t>
+  </si>
+  <si>
+    <t>TC_Amazon_Today's deals_009</t>
+  </si>
+  <si>
+    <t>Validate the amazon application to check Today's deals</t>
+  </si>
+  <si>
+    <t>TC_Amazon_Buy Again_010</t>
+  </si>
+  <si>
+    <t>Validate the amazon application for Buy Again feature</t>
+  </si>
+  <si>
+    <t>TC_Amazon_Sell_011</t>
+  </si>
+  <si>
+    <t>Validate the amazon application to Sell an item</t>
+  </si>
+  <si>
+    <t>TC_Amazon_Deliver to_012</t>
+  </si>
+  <si>
+    <t>Validate the amazon application to upadte delivery location</t>
+  </si>
+  <si>
+    <t>TC_Amazon_Payment_013</t>
+  </si>
+  <si>
+    <t>Validate the amazon application for payment options</t>
+  </si>
+  <si>
+    <t>TC_Amazon_Footer Links_014</t>
+  </si>
+  <si>
+    <t>Validate the amazon application for footer links</t>
+  </si>
+  <si>
+    <t>TC_Amazon_Log out_015</t>
+  </si>
+  <si>
+    <t>Validate the amazon application for Log out session</t>
   </si>
 </sst>
 </file>
@@ -387,7 +459,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -445,17 +517,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -508,13 +569,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -526,12 +590,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -544,6 +602,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -861,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9761F6C-F242-4EC2-AE99-913A20049DE8}">
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -881,7 +940,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -889,15 +948,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>76</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -905,26 +964,103 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>102</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>77</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
+      <c r="A7" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -936,7 +1072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F485A07-DC85-4F9F-B615-E1DF92A1C84C}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView topLeftCell="C5" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
       <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
@@ -997,13 +1133,13 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="19" t="s">
@@ -1021,16 +1157,16 @@
       <c r="H2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="18" t="s">
         <v>40</v>
       </c>
       <c r="M2" s="19" t="s">
@@ -1038,8 +1174,8 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
@@ -1050,15 +1186,15 @@
         <v>50</v>
       </c>
       <c r="H3" s="9"/>
-      <c r="I3" s="23"/>
+      <c r="I3" s="24"/>
       <c r="J3" s="19"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
       <c r="M3" s="19"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
@@ -1068,18 +1204,18 @@
       <c r="G4" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="23"/>
+      <c r="I4" s="24"/>
       <c r="J4" s="19"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
       <c r="M4" s="19"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
@@ -1089,16 +1225,16 @@
       <c r="G5" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="23"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="24"/>
       <c r="J5" s="19"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
       <c r="M5" s="19"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
@@ -1108,20 +1244,20 @@
       <c r="G6" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="21"/>
+      <c r="H6" s="22"/>
       <c r="I6" s="19" t="s">
         <v>55</v>
       </c>
       <c r="J6" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
       <c r="M6" s="19"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
@@ -1131,16 +1267,16 @@
       <c r="G7" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="21"/>
+      <c r="H7" s="22"/>
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
       <c r="M7" s="19"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
       <c r="E8" s="19"/>
@@ -1308,7 +1444,7 @@
       <c r="G16" t="s">
         <v>47</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="22" t="s">
         <v>53</v>
       </c>
       <c r="I16" s="19"/>
@@ -1329,7 +1465,7 @@
       <c r="G17" t="s">
         <v>48</v>
       </c>
-      <c r="H17" s="21"/>
+      <c r="H17" s="22"/>
       <c r="I17" s="19"/>
       <c r="J17" s="19"/>
       <c r="K17" s="19"/>
@@ -1355,7 +1491,7 @@
       <c r="M18" s="19"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="19" t="s">
@@ -1396,7 +1532,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
@@ -1417,7 +1553,7 @@
       <c r="M21" s="19"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
@@ -1438,7 +1574,7 @@
       <c r="M22" s="19"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
+      <c r="A23" s="18"/>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
       <c r="D23" s="19"/>
@@ -1457,7 +1593,7 @@
       <c r="M23" s="19"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="20"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
       <c r="D24" s="19"/>
@@ -1501,10 +1637,10 @@
         <v>32</v>
       </c>
       <c r="I26" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J26" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K26" s="19" t="s">
         <v>39</v>
@@ -1575,47 +1711,11 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="L2:L7"/>
-    <mergeCell ref="M2:M7"/>
-    <mergeCell ref="C2:C8"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="D2:D8"/>
-    <mergeCell ref="E2:E8"/>
-    <mergeCell ref="K2:K7"/>
-    <mergeCell ref="H4:H7"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="E15:E18"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="I2:I5"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J2:J5"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="K15:K18"/>
-    <mergeCell ref="L15:L18"/>
-    <mergeCell ref="M15:M18"/>
-    <mergeCell ref="M10:M13"/>
-    <mergeCell ref="L10:L13"/>
-    <mergeCell ref="K10:K13"/>
-    <mergeCell ref="I15:I18"/>
-    <mergeCell ref="J15:J18"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="C20:C24"/>
-    <mergeCell ref="D20:D24"/>
-    <mergeCell ref="E20:E24"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
     <mergeCell ref="K20:K24"/>
     <mergeCell ref="L20:L24"/>
     <mergeCell ref="M20:M24"/>
@@ -1626,11 +1726,47 @@
     <mergeCell ref="M26:M29"/>
     <mergeCell ref="I20:I24"/>
     <mergeCell ref="J20:J24"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="C20:C24"/>
+    <mergeCell ref="D20:D24"/>
+    <mergeCell ref="E20:E24"/>
+    <mergeCell ref="M15:M18"/>
+    <mergeCell ref="M10:M13"/>
+    <mergeCell ref="L10:L13"/>
+    <mergeCell ref="K10:K13"/>
+    <mergeCell ref="I15:I18"/>
+    <mergeCell ref="J15:J18"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="K15:K18"/>
+    <mergeCell ref="L15:L18"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="L2:L7"/>
+    <mergeCell ref="M2:M7"/>
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="D2:D8"/>
+    <mergeCell ref="E2:E8"/>
+    <mergeCell ref="K2:K7"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J2:J5"/>
+    <mergeCell ref="J6:J7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{099514FC-AA50-4279-B19D-F76E5E6146BB}"/>
@@ -1682,35 +1818,35 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="25"/>
+      <c r="B3" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
-      <c r="B3" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>87</v>
-      </c>
       <c r="E3" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1748,17 +1884,17 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="26" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="27"/>
+      <c r="B3" s="4" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="28"/>
-      <c r="B3" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1803,38 +1939,38 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="28" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="28"/>
+      <c r="B3" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
-      <c r="B3" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="29"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="29"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>62</v>
@@ -1872,7 +2008,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B2" s="15">
         <v>4</v>
@@ -1880,7 +2016,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B3" s="15">
         <v>2</v>
@@ -1896,7 +2032,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B5" s="15">
         <v>4</v>
@@ -1911,7 +2047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C78F78A-5CDC-4F23-8C7D-A533F8C3F620}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1923,7 +2059,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>66</v>
@@ -1931,23 +2067,23 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>68</v>
@@ -1955,10 +2091,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>98</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>